<commit_message>
nprice and stats update
</commit_message>
<xml_diff>
--- a/data_stefan/trt_mgmt.Amundson2.ReduceN.xlsx
+++ b/data_stefan/trt_mgmt.Amundson2.ReduceN.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://practicalfarmers.sharepoint.com/sites/Research/Shared Documents/CooperatorsProgram/ResearchProjects/FieldCrops/2022-2024/Can We Reduce N Rates and Improve ROI/2023/Cooperators/Alec_Rachel Amundson/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gina\Documents\_git-it\PFI_CanWeReduceN2\data_stefan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="85" documentId="8_{CEF81A76-9512-4113-B494-899867D1E05D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5278D033-44D8-4366-A04D-6E1BABC3722B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F3A7719-1CA1-4A06-9A2C-A3F053B42582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="4" xr2:uid="{BA11CEDC-CF96-4B69-AD2E-31C9B22CE6DC}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{BA11CEDC-CF96-4B69-AD2E-31C9B22CE6DC}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="4" r:id="rId1"/>
     <sheet name="trt" sheetId="1" r:id="rId2"/>
-    <sheet name="trt transposed" sheetId="6" r:id="rId3"/>
+    <sheet name="trt_transposed" sheetId="6" r:id="rId3"/>
     <sheet name="yld" sheetId="2" r:id="rId4"/>
     <sheet name="fieldhistory" sheetId="3" r:id="rId5"/>
     <sheet name="fieldactivities" sheetId="5" r:id="rId6"/>
@@ -482,7 +482,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -908,13 +908,13 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -934,7 +934,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -969,24 +969,24 @@
       <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="57.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" customWidth="1"/>
+    <col min="4" max="4" width="15.81640625" customWidth="1"/>
+    <col min="5" max="5" width="13.1796875" customWidth="1"/>
+    <col min="6" max="6" width="11.81640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C1" s="12" t="s">
         <v>11</v>
       </c>
@@ -997,7 +997,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30">
+    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
@@ -1014,7 +1014,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30">
+    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>18</v>
       </c>
@@ -1028,7 +1028,7 @@
         <v>44864</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="60">
+    <row r="4" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>20</v>
       </c>
@@ -1042,7 +1042,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="45">
+    <row r="5" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>23</v>
       </c>
@@ -1056,7 +1056,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="45">
+    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>25</v>
       </c>
@@ -1070,7 +1070,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="30">
+    <row r="7" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>27</v>
       </c>
@@ -1084,7 +1084,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="30">
+    <row r="8" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>30</v>
       </c>
@@ -1094,7 +1094,7 @@
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
     </row>
-    <row r="9" spans="1:5" ht="60">
+    <row r="9" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>32</v>
       </c>
@@ -1104,7 +1104,7 @@
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:5" ht="45">
+    <row r="10" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>34</v>
       </c>
@@ -1114,7 +1114,7 @@
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:5" ht="45">
+    <row r="11" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>36</v>
       </c>
@@ -1124,7 +1124,7 @@
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:5" ht="30">
+    <row r="12" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>38</v>
       </c>
@@ -1138,7 +1138,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="30">
+    <row r="13" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>40</v>
       </c>
@@ -1148,7 +1148,7 @@
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
     </row>
-    <row r="14" spans="1:5" ht="60">
+    <row r="14" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>42</v>
       </c>
@@ -1158,7 +1158,7 @@
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:5" ht="45">
+    <row r="15" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>44</v>
       </c>
@@ -1168,7 +1168,7 @@
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:5" ht="45">
+    <row r="16" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>46</v>
       </c>
@@ -1179,7 +1179,7 @@
       <c r="D16" s="7"/>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="1:5" ht="30">
+    <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>48</v>
       </c>
@@ -1193,7 +1193,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="30">
+    <row r="18" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>50</v>
       </c>
@@ -1207,7 +1207,7 @@
         <v>45049</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="60">
+    <row r="19" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>52</v>
       </c>
@@ -1224,7 +1224,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="45">
+    <row r="20" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>55</v>
       </c>
@@ -1238,7 +1238,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="45">
+    <row r="21" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>57</v>
       </c>
@@ -1252,7 +1252,7 @@
         <v>0.81</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="30">
+    <row r="22" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>59</v>
       </c>
@@ -1266,7 +1266,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="30">
+    <row r="23" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>61</v>
       </c>
@@ -1280,7 +1280,7 @@
         <v>45080</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="60">
+    <row r="24" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>63</v>
       </c>
@@ -1297,7 +1297,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="45">
+    <row r="25" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>66</v>
       </c>
@@ -1311,7 +1311,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="45">
+    <row r="26" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>68</v>
       </c>
@@ -1325,7 +1325,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>70</v>
       </c>
@@ -1339,7 +1339,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="30">
+    <row r="28" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>72</v>
       </c>
@@ -1353,7 +1353,7 @@
         <v>45114</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="60">
+    <row r="29" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>74</v>
       </c>
@@ -1370,7 +1370,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="45">
+    <row r="30" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>77</v>
       </c>
@@ -1384,7 +1384,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="45">
+    <row r="31" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>79</v>
       </c>
@@ -1408,16 +1408,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFE0DF5B-9BBC-41B5-B3AE-EE008367ECF1}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:I9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>81</v>
       </c>
@@ -1446,7 +1446,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>90</v>
       </c>
@@ -1475,7 +1475,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>90</v>
       </c>
@@ -1504,7 +1504,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>90</v>
       </c>
@@ -1533,7 +1533,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>90</v>
       </c>
@@ -1562,7 +1562,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>90</v>
       </c>
@@ -1591,7 +1591,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>90</v>
       </c>
@@ -1620,7 +1620,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>90</v>
       </c>
@@ -1649,7 +1649,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>90</v>
       </c>
@@ -1693,9 +1693,9 @@
       <selection sqref="A1:D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>83</v>
       </c>
@@ -1709,7 +1709,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>92</v>
       </c>
@@ -1723,7 +1723,7 @@
         <v>149.19999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>94</v>
       </c>
@@ -1737,7 +1737,7 @@
         <v>153.4</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>94</v>
       </c>
@@ -1751,7 +1751,7 @@
         <v>132.4</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>92</v>
       </c>
@@ -1765,7 +1765,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>94</v>
       </c>
@@ -1779,7 +1779,7 @@
         <v>144.9</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>92</v>
       </c>
@@ -1793,7 +1793,7 @@
         <v>164.1</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>92</v>
       </c>
@@ -1807,7 +1807,7 @@
         <v>163.4</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>94</v>
       </c>
@@ -1835,12 +1835,12 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="58.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="58.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>102</v>
       </c>
@@ -1851,7 +1851,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>105</v>
       </c>
@@ -1862,7 +1862,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>107</v>
       </c>
@@ -1873,7 +1873,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>109</v>
       </c>
@@ -1884,7 +1884,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>111</v>
       </c>
@@ -1895,7 +1895,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>113</v>
       </c>
@@ -1906,7 +1906,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>105</v>
       </c>
@@ -1917,7 +1917,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>107</v>
       </c>
@@ -1928,7 +1928,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>109</v>
       </c>
@@ -1939,7 +1939,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>111</v>
       </c>
@@ -1950,7 +1950,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>113</v>
       </c>
@@ -1961,7 +1961,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>105</v>
       </c>
@@ -1972,7 +1972,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>107</v>
       </c>
@@ -1983,7 +1983,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>109</v>
       </c>
@@ -1994,7 +1994,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>111</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>113</v>
       </c>
@@ -2016,7 +2016,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>105</v>
       </c>
@@ -2027,7 +2027,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>107</v>
       </c>
@@ -2038,7 +2038,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>109</v>
       </c>
@@ -2049,7 +2049,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>111</v>
       </c>
@@ -2060,7 +2060,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>113</v>
       </c>
@@ -2071,7 +2071,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
         <v>105</v>
       </c>
@@ -2082,7 +2082,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
         <v>107</v>
       </c>
@@ -2093,7 +2093,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>109</v>
       </c>
@@ -2104,7 +2104,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
         <v>111</v>
       </c>
@@ -2115,7 +2115,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
         <v>113</v>
       </c>
@@ -2126,7 +2126,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
         <v>105</v>
       </c>
@@ -2137,7 +2137,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
         <v>107</v>
       </c>
@@ -2148,7 +2148,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
         <v>109</v>
       </c>
@@ -2159,7 +2159,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
         <v>111</v>
       </c>
@@ -2170,7 +2170,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
         <v>113</v>
       </c>
@@ -2195,19 +2195,19 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="52.85546875" customWidth="1"/>
-    <col min="2" max="2" width="36.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.7109375" customWidth="1"/>
+    <col min="1" max="1" width="52.81640625" customWidth="1"/>
+    <col min="2" max="2" width="36.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C1" s="11" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>119</v>
       </c>
@@ -2215,7 +2215,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>120</v>
       </c>
@@ -2223,7 +2223,7 @@
         <v>1875</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>121</v>
       </c>
@@ -2231,7 +2231,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>122</v>
       </c>
@@ -2239,7 +2239,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>123</v>
       </c>
@@ -2247,7 +2247,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>125</v>
       </c>
@@ -2255,7 +2255,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30">
+    <row r="8" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>126</v>
       </c>
@@ -2263,7 +2263,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>127</v>
       </c>
@@ -2271,7 +2271,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>128</v>
       </c>
@@ -2282,7 +2282,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="30">
+    <row r="11" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>131</v>
       </c>
@@ -2290,7 +2290,7 @@
         <v>44803</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="30">
+    <row r="12" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>132</v>
       </c>
@@ -2298,7 +2298,7 @@
         <v>45050</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="30">
+    <row r="13" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>133</v>
       </c>
@@ -2309,7 +2309,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="30">
+    <row r="14" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>136</v>
       </c>
@@ -2317,7 +2317,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>137</v>
       </c>
@@ -2325,7 +2325,7 @@
         <v>45049</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>138</v>
       </c>
@@ -2333,7 +2333,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>139</v>
       </c>
@@ -2341,7 +2341,7 @@
         <v>32500</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>140</v>
       </c>
@@ -2349,7 +2349,7 @@
         <v>45204</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>141</v>
       </c>
@@ -2357,7 +2357,7 @@
         <v>5.0599999999999996</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="30">
+    <row r="20" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>142</v>
       </c>
@@ -2368,49 +2368,49 @@
         <v>143</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="6" t="s">
         <v>144</v>
       </c>
       <c r="B21" s="9"/>
       <c r="C21" s="4"/>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="6" t="s">
         <v>144</v>
       </c>
       <c r="B22" s="9"/>
       <c r="C22" s="4"/>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="6" t="s">
         <v>144</v>
       </c>
       <c r="B23" s="10"/>
       <c r="C23" s="4"/>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="6" t="s">
         <v>144</v>
       </c>
       <c r="B24" s="10"/>
       <c r="C24" s="4"/>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="6" t="s">
         <v>144</v>
       </c>
       <c r="B25" s="10"/>
       <c r="C25" s="4"/>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="6" t="s">
         <v>144</v>
       </c>
       <c r="B26" s="10"/>
       <c r="C26" s="4"/>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="6" t="s">
         <v>144</v>
       </c>
@@ -2423,15 +2423,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005BE0433617A9764B83875192EFA7799D" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e9cbbb3ca604aca823f56b8e4b22fe47">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="170271cd-7847-44f3-81b8-91d966c9299e" xmlns:ns3="5c162411-790a-4090-8516-4c29411b79ed" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ad1e2fcf57f1a99c88c4998cae0ad6c1" ns2:_="" ns3:_="">
     <xsd:import namespace="170271cd-7847-44f3-81b8-91d966c9299e"/>
@@ -2666,6 +2657,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2678,13 +2678,39 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8474E227-F805-43E6-A496-5B3375444D2F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D518865-79B6-4792-953D-CEB2C848CEFF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="170271cd-7847-44f3-81b8-91d966c9299e"/>
+    <ds:schemaRef ds:uri="5c162411-790a-4090-8516-4c29411b79ed"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D518865-79B6-4792-953D-CEB2C848CEFF}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8474E227-F805-43E6-A496-5B3375444D2F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56253EEC-E66A-436A-B529-C957B1E9FD22}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56253EEC-E66A-436A-B529-C957B1E9FD22}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5c162411-790a-4090-8516-4c29411b79ed"/>
+    <ds:schemaRef ds:uri="170271cd-7847-44f3-81b8-91d966c9299e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>